<commit_message>
Added prices to BoM
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom-v008.xlsx
+++ b/Bill of Materials/core-bom-v008.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Quote sheet v0.0.8" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$G$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$H$27</definedName>
     <definedName name="bom" localSheetId="0">BOM!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="143">
   <si>
     <t>Part</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/KMR211GLFS/401-1426-1-ND/550461</t>
   </si>
   <si>
@@ -477,13 +474,81 @@
   </si>
   <si>
     <t>0Ω</t>
+  </si>
+  <si>
+    <t>DigiKey Link</t>
+  </si>
+  <si>
+    <t>Taobao Link</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.1.pBjcgl&amp;id=10605978811</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.1.sDPMv0&amp;id=5913218207</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.59.xxVeAY&amp;id=16690855349</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.21.Zvi13g&amp;id=17377012127</t>
+  </si>
+  <si>
+    <t>http://detail.tmall.com/item.htm?spm=a230r.1.14.42.nwHrUU&amp;id=14139679780</t>
+  </si>
+  <si>
+    <t>http://detail.tmall.com/item.htm?spm=a230r.1.14.28.HWbOvn&amp;id=15456269891</t>
+  </si>
+  <si>
+    <t>http://detail.tmall.com/item.htm?spm=a230r.1.14.1.mIn2bB&amp;id=17921640239</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.29.on1ODT&amp;id=16348539730</t>
+  </si>
+  <si>
+    <t>6.5mm x 2.8mm</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.62.jgHr9v&amp;id=13004811346</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.1.ftfZaL&amp;id=10614261731</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.1.JxpGm6&amp;id=21970968624</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=2013.1.w3956858894.1.emTPiQ&amp;id=12920296504</t>
+  </si>
+  <si>
+    <t>http://item.taobao.com/item.htm?spm=a230r.1.14.34.tpoElm&amp;id=15691378326</t>
+  </si>
+  <si>
+    <t>Price (CNY)</t>
+  </si>
+  <si>
+    <t>Price (USD)</t>
+  </si>
+  <si>
+    <t>Total Price (USD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,145 +726,151 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="109">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="109" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="109" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="109">
+  <cellStyles count="112">
+    <cellStyle name="Currency" xfId="109" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -854,6 +925,7 @@
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -908,6 +980,7 @@
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1241,11 +1314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1254,13 +1326,14 @@
     <col min="2" max="2" width="41.83203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="28.5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="7"/>
-    <col min="7" max="7" width="11.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="7"/>
+    <col min="5" max="5" width="10.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="7"/>
+    <col min="8" max="8" width="11.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="20" customFormat="1">
+    <row r="1" spans="1:11" s="20" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1274,16 +1347,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="F1" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" customFormat="1" hidden="1">
+      <c r="I1" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1294,62 +1379,103 @@
         <v>24</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
+        <v>134</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1">
+      <c r="H2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="7">
+        <v>2</v>
+      </c>
+      <c r="J2" s="22">
+        <f>I2/6.178</f>
+        <v>0.32372936225315635</v>
+      </c>
+      <c r="K2" s="22">
+        <f>J2*G2</f>
+        <v>0.32372936225315635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>113</v>
+        <v>102</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="J3" s="22">
+        <f t="shared" ref="J3:J26" si="0">I3/6.178</f>
+        <v>0.40466170281644548</v>
+      </c>
+      <c r="K3" s="22">
+        <f t="shared" ref="K3:K26" si="1">J3*G3</f>
+        <v>0.80932340563289096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="7">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1">
-      <c r="A4" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="F4" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="7">
         <v>3</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="J4" s="22">
+        <f t="shared" si="0"/>
+        <v>4.8559404337973455E-2</v>
+      </c>
+      <c r="K4" s="22">
+        <f t="shared" si="1"/>
+        <v>0.14567821301392037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -1358,16 +1484,27 @@
         <v>18</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="7">
+        <v>68</v>
+      </c>
+      <c r="G5" s="7">
         <v>7</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J5" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K5" s="22">
+        <f t="shared" si="1"/>
+        <v>6.7983166073162835E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
@@ -1378,18 +1515,29 @@
         <v>18</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="7">
+        <v>68</v>
+      </c>
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J6" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K6" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>6</v>
@@ -1398,21 +1546,32 @@
         <v>18</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="7">
+        <v>68</v>
+      </c>
+      <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J7" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K7" s="22">
+        <f t="shared" si="1"/>
+        <v>1.9423761735189383E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>7</v>
@@ -1420,14 +1579,28 @@
       <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" hidden="1">
+      <c r="H8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J8" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K8" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -1435,38 +1608,61 @@
         <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="22">
+        <f t="shared" si="0"/>
+        <v>8.0932340563289087E-2</v>
+      </c>
+      <c r="K9" s="22">
+        <f t="shared" si="1"/>
+        <v>8.0932340563289087E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" customFormat="1">
-      <c r="A10" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>2</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="22">
+        <f t="shared" si="0"/>
+        <v>1.618646811265782E-2</v>
+      </c>
+      <c r="K10" s="22">
+        <f t="shared" si="1"/>
+        <v>3.2372936225315639E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
         <v>31</v>
       </c>
@@ -1474,60 +1670,100 @@
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="7">
+        <v>68</v>
+      </c>
+      <c r="G11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J11" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K11" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="7">
+        <f>6/100</f>
+        <v>0.06</v>
+      </c>
+      <c r="J12" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K12" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" customFormat="1">
-      <c r="A13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7">
+        <v>68</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="7">
         <v>3</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1">
+      <c r="H13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="7">
+        <f>1.5/20</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J13" s="22">
+        <f t="shared" si="0"/>
+        <v>1.2139851084493364E-2</v>
+      </c>
+      <c r="K13" s="22">
+        <f t="shared" si="1"/>
+        <v>3.6419553253480091E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
@@ -1540,16 +1776,30 @@
       <c r="D14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="7">
         <v>1</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="J14" s="22">
+        <f t="shared" si="0"/>
+        <v>2.4279702168986728E-2</v>
+      </c>
+      <c r="K14" s="22">
+        <f t="shared" si="1"/>
+        <v>2.4279702168986728E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>11</v>
@@ -1558,16 +1808,27 @@
         <v>20</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="7">
+        <v>68</v>
+      </c>
+      <c r="G15" s="7">
         <v>4</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J15" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K15" s="22">
+        <f t="shared" si="1"/>
+        <v>3.8847523470378766E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
@@ -1578,16 +1839,27 @@
         <v>20</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="7">
+        <v>68</v>
+      </c>
+      <c r="G16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J16" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K16" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
@@ -1598,18 +1870,29 @@
         <v>20</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="7">
+        <v>68</v>
+      </c>
+      <c r="G17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J17" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K17" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>21</v>
@@ -1618,18 +1901,29 @@
         <v>20</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="7">
+        <v>68</v>
+      </c>
+      <c r="G18" s="7">
         <v>2</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J18" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K18" s="22">
+        <f t="shared" si="1"/>
+        <v>1.9423761735189383E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>42</v>
@@ -1638,18 +1932,29 @@
         <v>20</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="7">
+        <v>68</v>
+      </c>
+      <c r="G19" s="7">
         <v>1</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J19" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K19" s="22">
+        <f t="shared" si="1"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>10</v>
@@ -1658,36 +1963,61 @@
         <v>20</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="7">
+        <v>68</v>
+      </c>
+      <c r="G20" s="7">
         <v>5</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1">
+      <c r="H20" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="J20" s="22">
+        <f t="shared" si="0"/>
+        <v>9.7118808675946914E-3</v>
+      </c>
+      <c r="K20" s="22">
+        <f t="shared" si="1"/>
+        <v>4.8559404337973455E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" customFormat="1" hidden="1">
+      <c r="H21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="22">
+        <f t="shared" si="0"/>
+        <v>0.12949174490126256</v>
+      </c>
+      <c r="K21" s="22">
+        <f t="shared" si="1"/>
+        <v>0.12949174490126256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
@@ -1695,25 +2025,31 @@
         <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
+      <c r="G22" s="7">
         <v>1</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1">
+      <c r="H22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="22">
+        <v>9</v>
+      </c>
+      <c r="K22" s="22">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>47</v>
@@ -1721,55 +2057,96 @@
       <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="7">
         <v>1</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1">
+      <c r="H23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="7">
+        <v>11.1</v>
+      </c>
+      <c r="J23" s="22">
+        <f t="shared" si="0"/>
+        <v>1.7966979605050177</v>
+      </c>
+      <c r="K23" s="22">
+        <f t="shared" si="1"/>
+        <v>1.7966979605050177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="F24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="7">
         <v>1</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" customFormat="1" hidden="1">
+      <c r="H24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="J24" s="22">
+        <f t="shared" si="0"/>
+        <v>0.52606021366137912</v>
+      </c>
+      <c r="K24" s="22">
+        <f t="shared" si="1"/>
+        <v>0.52606021366137912</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7">
+      <c r="F25" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" s="7">
         <v>1</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" customFormat="1" hidden="1">
+      <c r="H25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="J25" s="22">
+        <f t="shared" si="0"/>
+        <v>5.665263839430236E-2</v>
+      </c>
+      <c r="K25" s="22">
+        <f t="shared" si="1"/>
+        <v>5.665263839430236E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="7" t="s">
         <v>49</v>
       </c>
@@ -1780,24 +2157,37 @@
         <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7">
+        <v>80</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="7">
         <v>1</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>83</v>
+      <c r="H26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0.88</v>
+      </c>
+      <c r="J26" s="22">
+        <f t="shared" si="0"/>
+        <v>0.14244091939138881</v>
+      </c>
+      <c r="K26" s="22">
+        <f t="shared" si="1"/>
+        <v>0.14244091939138881</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="K28" s="21">
+        <f>SUM(K2:K26)</f>
+        <v>13.366299773389446</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G27">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Need"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H27"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1839,25 +2229,25 @@
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="13" thickBot="1">
       <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="N2" s="2">
         <f ca="1">NOW()</f>
-        <v>41373.577706365744</v>
+        <v>41382.461860995369</v>
       </c>
     </row>
     <row r="3" spans="2:14">
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
@@ -1869,7 +2259,7 @@
     </row>
     <row r="4" spans="2:14" ht="16" thickBot="1">
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -1882,10 +2272,10 @@
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
@@ -1897,7 +2287,7 @@
     </row>
     <row r="6" spans="2:14" ht="16" thickBot="1">
       <c r="B6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
@@ -1910,10 +2300,10 @@
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
@@ -1925,7 +2315,7 @@
     </row>
     <row r="8" spans="2:14" ht="16" thickBot="1">
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
@@ -1954,19 +2344,19 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="2:14" s="1" customFormat="1" ht="12">
       <c r="B11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>1</v>
@@ -1976,40 +2366,40 @@
         <v>3</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="15">
         <v>10</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L12" s="15">
         <v>2.5</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N12" s="15">
         <f>J12*L12</f>
@@ -2018,28 +2408,28 @@
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J13" s="15">
         <v>100</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="15">
         <v>0.8</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" ref="N13:N30" si="0">J13*L13</f>
@@ -2048,7 +2438,7 @@
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
@@ -2057,19 +2447,19 @@
         <v>5</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14" s="15">
         <v>1000</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L14" s="15">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="0"/>
@@ -2087,19 +2477,19 @@
         <v>26</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15" s="15">
         <v>1000</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" s="15">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="0"/>
@@ -2108,7 +2498,7 @@
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>18</v>
@@ -2117,19 +2507,19 @@
         <v>6</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J16" s="15">
         <v>1000</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L16" s="15">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="0"/>
@@ -2144,7 +2534,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>28</v>
@@ -2153,13 +2543,13 @@
         <v>10</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="15">
         <v>2</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="0"/>
@@ -2171,25 +2561,25 @@
         <v>29</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="15">
         <v>10</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" s="15">
         <v>1.5</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="0"/>
@@ -2201,25 +2591,25 @@
         <v>31</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J19" s="15">
         <v>10</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L19" s="15">
         <v>0.8</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" si="0"/>
@@ -2231,25 +2621,25 @@
         <v>33</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J20" s="15">
         <v>10</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L20" s="15">
         <v>2.5</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="0"/>
@@ -2273,13 +2663,13 @@
         <v>10</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L21" s="15">
         <v>2</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N21" s="15">
         <f t="shared" si="0"/>
@@ -2288,7 +2678,7 @@
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>20</v>
@@ -2297,19 +2687,19 @@
         <v>11</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J22" s="15">
         <v>1000</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L22" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="0"/>
@@ -2327,19 +2717,19 @@
         <v>22</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J23" s="15">
         <v>1000</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L23" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="0"/>
@@ -2357,19 +2747,19 @@
         <v>40</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J24" s="15">
         <v>1000</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L24" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N24" s="15">
         <f t="shared" si="0"/>
@@ -2378,7 +2768,7 @@
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>20</v>
@@ -2387,19 +2777,19 @@
         <v>21</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J25" s="15">
         <v>1000</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L25" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N25" s="15">
         <f t="shared" si="0"/>
@@ -2417,19 +2807,19 @@
         <v>42</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" s="15">
         <v>1000</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L26" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N26" s="15">
         <f t="shared" si="0"/>
@@ -2438,7 +2828,7 @@
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>20</v>
@@ -2447,19 +2837,19 @@
         <v>10</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J27" s="15">
         <v>1000</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L27" s="15">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N27" s="15">
         <f t="shared" si="0"/>
@@ -2471,10 +2861,10 @@
         <v>12</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>43</v>
@@ -2483,13 +2873,13 @@
         <v>10</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L28" s="15">
         <v>4.8</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N28" s="15">
         <f t="shared" si="0"/>
@@ -2501,10 +2891,10 @@
         <v>46</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>15</v>
@@ -2513,13 +2903,13 @@
         <v>10</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L29" s="15">
         <v>22</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N29" s="15">
         <f t="shared" si="0"/>
@@ -2531,25 +2921,25 @@
         <v>48</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="J30" s="15">
         <v>10</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L30" s="15">
         <v>7</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N30" s="15">
         <f t="shared" si="0"/>
@@ -2570,7 +2960,7 @@
     </row>
     <row r="33" spans="12:14">
       <c r="L33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N33" s="18">
         <f>SUM(N12:N30)</f>
@@ -2579,7 +2969,7 @@
     </row>
     <row r="34" spans="12:14">
       <c r="L34" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N34" s="19"/>
     </row>
@@ -2598,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -2625,25 +3015,25 @@
   <sheetData>
     <row r="2" spans="2:14" s="1" customFormat="1" ht="13" thickBot="1">
       <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="N2" s="2">
         <f ca="1">NOW()</f>
-        <v>41373.577706365744</v>
+        <v>41382.461860995369</v>
       </c>
     </row>
     <row r="3" spans="2:14">
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
@@ -2655,7 +3045,7 @@
     </row>
     <row r="4" spans="2:14" ht="16" thickBot="1">
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -2668,10 +3058,10 @@
     </row>
     <row r="5" spans="2:14">
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10"/>
@@ -2683,7 +3073,7 @@
     </row>
     <row r="6" spans="2:14" ht="16" thickBot="1">
       <c r="B6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
@@ -2696,10 +3086,10 @@
     </row>
     <row r="7" spans="2:14">
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
@@ -2711,7 +3101,7 @@
     </row>
     <row r="8" spans="2:14" ht="16" thickBot="1">
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="13"/>
@@ -2740,19 +3130,19 @@
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="2:14" s="1" customFormat="1" ht="12">
       <c r="B11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>1</v>
@@ -2762,19 +3152,19 @@
         <v>3</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>18</v>
@@ -2783,17 +3173,17 @@
         <v>5</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J12" s="15">
         <v>4000</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N12" s="15">
         <f>J12*L12</f>
@@ -2811,17 +3201,17 @@
         <v>26</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J13" s="15">
         <v>100</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" ref="N13:N26" si="0">J13*L13</f>
@@ -2830,7 +3220,7 @@
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
@@ -2839,17 +3229,17 @@
         <v>6</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J14" s="15">
         <v>100</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N14" s="15">
         <f t="shared" si="0"/>
@@ -2864,7 +3254,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>28</v>
@@ -2873,11 +3263,11 @@
         <v>10</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N15" s="15">
         <f t="shared" si="0"/>
@@ -2889,23 +3279,23 @@
         <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" s="15">
         <v>100</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N16" s="15">
         <f t="shared" si="0"/>
@@ -2917,23 +3307,23 @@
         <v>33</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J17" s="15">
         <v>100</v>
       </c>
       <c r="K17" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N17" s="15">
         <f t="shared" si="0"/>
@@ -2942,26 +3332,26 @@
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J18" s="15">
         <v>100</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N18" s="15">
         <f t="shared" si="0"/>
@@ -2970,24 +3360,24 @@
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="H19" s="17"/>
       <c r="J19" s="15">
         <v>10</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N19" s="15">
         <f t="shared" ref="N19" si="1">J19*L19</f>
@@ -2996,7 +3386,7 @@
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>20</v>
@@ -3005,17 +3395,17 @@
         <v>11</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J20" s="15">
         <v>4000</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L20" s="15"/>
       <c r="M20" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N20" s="15">
         <f t="shared" si="0"/>
@@ -3033,17 +3423,17 @@
         <v>22</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J21" s="15">
         <v>100</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N21" s="15">
         <f t="shared" si="0"/>
@@ -3061,17 +3451,17 @@
         <v>40</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" s="15">
         <v>100</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N22" s="15">
         <f t="shared" si="0"/>
@@ -3080,7 +3470,7 @@
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>20</v>
@@ -3089,17 +3479,17 @@
         <v>21</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J23" s="15">
         <v>100</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N23" s="15">
         <f t="shared" si="0"/>
@@ -3108,7 +3498,7 @@
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>20</v>
@@ -3117,17 +3507,17 @@
         <v>42</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J24" s="15">
         <v>100</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L24" s="15"/>
       <c r="M24" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N24" s="15">
         <f t="shared" si="0"/>
@@ -3139,16 +3529,16 @@
         <v>20</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J25" s="15">
         <v>4000</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L25" s="15"/>
       <c r="M25" s="16"/>
@@ -3159,7 +3549,7 @@
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>20</v>
@@ -3168,17 +3558,17 @@
         <v>10</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J26" s="15">
         <v>4000</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L26" s="15"/>
       <c r="M26" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N26" s="15">
         <f t="shared" si="0"/>
@@ -3199,7 +3589,7 @@
     </row>
     <row r="29" spans="2:14">
       <c r="L29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N29" s="18">
         <f>SUM(N12:N26)</f>
@@ -3208,7 +3598,7 @@
     </row>
     <row r="30" spans="2:14">
       <c r="L30" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N30" s="19"/>
     </row>

</xml_diff>